<commit_message>
updated data with new pop 18 and rates vacc limited to 100
</commit_message>
<xml_diff>
--- a/population/Statewise Projected Population 18 and above for 2021.xlsx
+++ b/population/Statewise Projected Population 18 and above for 2021.xlsx
@@ -1,31 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rakesh mishra\Dropbox\PC\Desktop\Covid-19 Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/16f1c7c3db740efb/UNICEF/india_co/1st_exp/population/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4693AE4A-530A-4271-988B-3EC82F61FB2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{4693AE4A-530A-4271-988B-3EC82F61FB2A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{E5AB10B0-222F-4198-BCDC-11374AE8527C}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{87033293-4B09-4E6A-8B9D-2F5B58913612}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{87033293-4B09-4E6A-8B9D-2F5B58913612}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t xml:space="preserve">States </t>
   </si>
@@ -148,6 +157,9 @@
   </si>
   <si>
     <t>Projected Population (18+) 2021 (in '000)</t>
+  </si>
+  <si>
+    <t>entero de ...</t>
   </si>
 </sst>
 </file>
@@ -219,7 +231,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -515,20 +527,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D3BBC2E-459E-452A-8CA9-7C231BC235A0}">
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -538,8 +551,11 @@
       <c r="C1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -550,8 +566,12 @@
         <f t="shared" ref="C2:C39" si="0">B2*1000</f>
         <v>369959.02114104934</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E2" s="2">
+        <f>INT(C2)</f>
+        <v>369959</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -562,8 +582,12 @@
         <f t="shared" si="0"/>
         <v>39521000</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E3" s="2">
+        <f t="shared" ref="E3:E39" si="1">INT(C3)</f>
+        <v>39521000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -574,8 +598,12 @@
         <f t="shared" si="0"/>
         <v>1154894.4174816655</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E4" s="2">
+        <f t="shared" si="1"/>
+        <v>1154894</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -586,8 +614,12 @@
         <f t="shared" si="0"/>
         <v>23658000</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E5" s="2">
+        <f t="shared" si="1"/>
+        <v>23658000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -598,8 +630,12 @@
         <f t="shared" si="0"/>
         <v>73449000</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E6" s="2">
+        <f t="shared" si="1"/>
+        <v>73449000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -610,8 +646,12 @@
         <f t="shared" si="0"/>
         <v>564679.06803416554</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E7" s="2">
+        <f t="shared" si="1"/>
+        <v>564679</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -622,8 +662,12 @@
         <f t="shared" si="0"/>
         <v>19650000</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E8" s="2">
+        <f t="shared" si="1"/>
+        <v>19650000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -634,8 +678,12 @@
         <f t="shared" si="0"/>
         <v>509406.70171997161</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E9" s="2">
+        <f t="shared" si="1"/>
+        <v>509406</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -646,8 +694,12 @@
         <f t="shared" si="0"/>
         <v>451268.73905108374</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E10" s="2">
+        <f t="shared" si="1"/>
+        <v>451268</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -658,8 +710,12 @@
         <f t="shared" si="0"/>
         <v>15080000</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E11" s="2">
+        <f t="shared" si="1"/>
+        <v>15080000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -670,8 +726,12 @@
         <f t="shared" si="0"/>
         <v>1509865.6039937511</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E12" s="2">
+        <f t="shared" si="1"/>
+        <v>1509865</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -682,8 +742,12 @@
         <f t="shared" si="0"/>
         <v>48908000</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E13" s="2">
+        <f t="shared" si="1"/>
+        <v>48908000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -694,8 +758,12 @@
         <f t="shared" si="0"/>
         <v>20581000</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E14" s="2">
+        <f t="shared" si="1"/>
+        <v>20581000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -706,8 +774,12 @@
         <f t="shared" si="0"/>
         <v>5523000</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E15" s="2">
+        <f t="shared" si="1"/>
+        <v>5523000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -718,8 +790,12 @@
         <f t="shared" si="0"/>
         <v>9408000</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E16" s="2">
+        <f t="shared" si="1"/>
+        <v>9408000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -730,8 +806,12 @@
         <f t="shared" si="0"/>
         <v>24863000</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E17" s="2">
+        <f t="shared" si="1"/>
+        <v>24863000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -742,8 +822,12 @@
         <f t="shared" si="0"/>
         <v>48917000</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E18" s="2">
+        <f t="shared" si="1"/>
+        <v>48917000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -754,8 +838,12 @@
         <f t="shared" si="0"/>
         <v>26708000</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E19" s="2">
+        <f t="shared" si="1"/>
+        <v>26708000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -766,8 +854,12 @@
         <f t="shared" si="0"/>
         <v>269070.13434650662</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E20" s="2">
+        <f t="shared" si="1"/>
+        <v>269070</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -778,8 +870,12 @@
         <f t="shared" si="0"/>
         <v>61671.539575432565</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E21" s="2">
+        <f t="shared" si="1"/>
+        <v>61671</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -790,8 +886,12 @@
         <f t="shared" si="0"/>
         <v>54949000</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E22" s="2">
+        <f t="shared" si="1"/>
+        <v>54949000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -802,8 +902,12 @@
         <f t="shared" si="0"/>
         <v>91435000</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E23" s="2">
+        <f t="shared" si="1"/>
+        <v>91435000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -814,8 +918,12 @@
         <f t="shared" si="0"/>
         <v>2646595.6376151806</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E24" s="2">
+        <f t="shared" si="1"/>
+        <v>2646595</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -826,8 +934,12 @@
         <f t="shared" si="0"/>
         <v>2304783.4406585847</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E25" s="2">
+        <f t="shared" si="1"/>
+        <v>2304783</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -838,8 +950,12 @@
         <f t="shared" si="0"/>
         <v>981667.05496279919</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E26" s="2">
+        <f t="shared" si="1"/>
+        <v>981667</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -850,8 +966,12 @@
         <f t="shared" si="0"/>
         <v>1683759.1392458081</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E27" s="2">
+        <f t="shared" si="1"/>
+        <v>1683759</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -862,8 +982,12 @@
         <f t="shared" si="0"/>
         <v>31369000</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E28" s="2">
+        <f t="shared" si="1"/>
+        <v>31369000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -874,8 +998,12 @@
         <f t="shared" si="0"/>
         <v>1471320.4312022822</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E29" s="2">
+        <f t="shared" si="1"/>
+        <v>1471320</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -886,8 +1014,12 @@
         <f t="shared" si="0"/>
         <v>22738000</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E30" s="2">
+        <f t="shared" si="1"/>
+        <v>22738000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -898,8 +1030,12 @@
         <f t="shared" si="0"/>
         <v>51509000</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E31" s="2">
+        <f t="shared" si="1"/>
+        <v>51509000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -910,8 +1046,12 @@
         <f t="shared" si="0"/>
         <v>588565.7634998397</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E32" s="2">
+        <f t="shared" si="1"/>
+        <v>588565</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -922,8 +1062,12 @@
         <f t="shared" si="0"/>
         <v>57891000</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E33" s="2">
+        <f t="shared" si="1"/>
+        <v>57891000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -934,8 +1078,12 @@
         <f t="shared" si="0"/>
         <v>27767000</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E34" s="2">
+        <f t="shared" si="1"/>
+        <v>27767000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -946,8 +1094,12 @@
         <f t="shared" si="0"/>
         <v>3557493.3074718527</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E35" s="2">
+        <f t="shared" si="1"/>
+        <v>3557493</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -958,8 +1110,12 @@
         <f t="shared" si="0"/>
         <v>147424000</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E36" s="2">
+        <f t="shared" si="1"/>
+        <v>147424000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -970,8 +1126,12 @@
         <f t="shared" si="0"/>
         <v>8063000</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E37" s="2">
+        <f t="shared" si="1"/>
+        <v>8063000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -982,8 +1142,12 @@
         <f t="shared" si="0"/>
         <v>72651000</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E38" s="2">
+        <f t="shared" si="1"/>
+        <v>72651000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
         <v>38</v>
       </c>
@@ -993,6 +1157,10 @@
       </c>
       <c r="C39" s="4">
         <f t="shared" si="0"/>
+        <v>940187000</v>
+      </c>
+      <c r="E39" s="2">
+        <f t="shared" si="1"/>
         <v>940187000</v>
       </c>
     </row>

</xml_diff>